<commit_message>
Excel Integration To Measurement
</commit_message>
<xml_diff>
--- a/LogBook.xlsx
+++ b/LogBook.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Freq</t>
+          <t>MWFreq</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Power</t>
+          <t>MWPow</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Calib</t>
+          <t>CalibN</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -508,59 +508,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>TEsting Excel2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Test</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>0/150/0.4</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>3000.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+          <t>calibMagnet.dat</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>/</t>
@@ -568,71 +564,67 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>LockIn</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Excel 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>&lt;PyQt5.QtWidgets.QLineEdit object at 0x000001237F4248B0&gt;/&lt;PyQt5.QtWidgets.QLineEdit object at 0x000001237F424940&gt;/0.4</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>3000.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+          <t>calibMagnet.dat</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>/</t>
@@ -640,10 +632,226 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>LockIn</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>/</t>
         </is>

</xml_diff>